<commit_message>
Añadidos cambios en la implementacion del modelo con la nueva funcionalidad y modificada carga del fichero excel
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13245" windowHeight="6075"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="16185" windowHeight="5910"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -12,9 +12,6 @@
   <calcPr calcId="0" concurrentCalc="0"/>
   <oleSize ref="A1"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -26,59 +23,20 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Nombre</t>
   </si>
   <si>
-    <t>90500084Y</t>
-  </si>
-  <si>
-    <t>19160962F</t>
-  </si>
-  <si>
-    <t>09940449X</t>
-  </si>
-  <si>
-    <t>C/ Federico García Lorca 2</t>
-  </si>
-  <si>
-    <t>C/ Real Oviedo 2</t>
-  </si>
-  <si>
-    <t>Av. De la Constitución 8</t>
-  </si>
-  <si>
-    <t>Apellidos</t>
-  </si>
-  <si>
     <t>Juan</t>
   </si>
   <si>
-    <t>Torres Pardo</t>
-  </si>
-  <si>
     <t>Luis</t>
   </si>
   <si>
-    <t>López Fernando</t>
-  </si>
-  <si>
     <t>Ana</t>
   </si>
   <si>
-    <t>DNI</t>
-  </si>
-  <si>
-    <t>Fecha nacimiento</t>
-  </si>
-  <si>
-    <t>Nacionalidad</t>
-  </si>
-  <si>
-    <t>Español</t>
-  </si>
-  <si>
     <t>Correo electrónico</t>
   </si>
   <si>
@@ -91,13 +49,25 @@
     <t>ana@example.com</t>
   </si>
   <si>
-    <t>Dirección postal</t>
+    <t>Localizacion</t>
+  </si>
+  <si>
+    <t>105.70.56</t>
+  </si>
+  <si>
+    <t>109.8.9</t>
+  </si>
+  <si>
+    <t>Identificador</t>
+  </si>
+  <si>
+    <t>Tipo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -139,9 +109,9 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -203,7 +173,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -238,7 +208,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -415,7 +385,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -425,8 +395,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,92 +411,69 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="2">
-        <v>31330</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="2">
-        <v>25629</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3">
         <v>2</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="3">
-        <v>21916</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="4">
         <v>3</v>
       </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Adaptado el CSV a la aplicación (leer descripción)
Ahora la aplicación puede cargar y procesar correctamente el fichero
maestro CSV (antes la aplicación solo almacenaba el contenido en una
lista), donde se almacenan los tipos de agentes de la aplicación. 
Se han arreglado también ciertos fallos de versiones anteriores, tales
como etiquetas ID repetidas, hashcode e equals mal formados, entre
alguna otra cosa.

Se han refactorizado las clases del proyecto. Cualquier "Citizen" pasa a
ser "Agent".

Se ha modificado ligeramente la forma de ejecutar la aplicación, siendo
obligatorio, en estos momentos, pasar tres parámetros a la función main.
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PabloD\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7680"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12900" windowHeight="3480"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>Nombre</t>
   </si>
@@ -69,6 +65,57 @@
   </si>
   <si>
     <t>Pablo Díaz</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>Sensor</t>
+  </si>
+  <si>
+    <t>Entity</t>
+  </si>
+  <si>
+    <t>59019237X</t>
+  </si>
+  <si>
+    <t>57104958S</t>
+  </si>
+  <si>
+    <t>10573947Y</t>
+  </si>
+  <si>
+    <t>58429367Y</t>
+  </si>
+  <si>
+    <t>sensor1@sensor.com</t>
+  </si>
+  <si>
+    <t>102.00.1</t>
+  </si>
+  <si>
+    <t>Sensor1</t>
+  </si>
+  <si>
+    <t>Sensor2</t>
+  </si>
+  <si>
+    <t>999.1.120</t>
+  </si>
+  <si>
+    <t>sensor2@sensor.com</t>
+  </si>
+  <si>
+    <t>EntityX100</t>
+  </si>
+  <si>
+    <t>entity@entity.com</t>
+  </si>
+  <si>
+    <t>192.168.0.25</t>
+  </si>
+  <si>
+    <t>Entity1</t>
   </si>
 </sst>
 </file>
@@ -113,9 +160,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -431,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,7 +498,7 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -466,11 +515,11 @@
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -483,11 +532,11 @@
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -500,11 +549,11 @@
       <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4">
-        <v>3</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
+      <c r="D4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -514,11 +563,62 @@
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D5">
-        <v>4</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="2">
+        <v>3000</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="2">
+        <v>19800</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -527,6 +627,9 @@
     <hyperlink ref="C3" r:id="rId2"/>
     <hyperlink ref="C4" r:id="rId3"/>
     <hyperlink ref="C5" r:id="rId4"/>
+    <hyperlink ref="C6" r:id="rId5"/>
+    <hyperlink ref="C7" r:id="rId6"/>
+    <hyperlink ref="C8" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Mejorados las pruebas sobre la base de datos y el fichero Excel
Se han añadido nuevas pruebas del sistema, teniendo en cuenta los nuevos 
requisitos.
</commit_message>
<xml_diff>
--- a/src/test/resources/test.xlsx
+++ b/src/test/resources/test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12900" windowHeight="3480"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13035" windowHeight="2700"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t>Nombre</t>
   </si>
@@ -116,6 +116,21 @@
   </si>
   <si>
     <t>Entity1</t>
+  </si>
+  <si>
+    <t>Sin email</t>
+  </si>
+  <si>
+    <t>100.0.11</t>
+  </si>
+  <si>
+    <t>1111111X</t>
+  </si>
+  <si>
+    <t>Pepe</t>
+  </si>
+  <si>
+    <t>21487463Y</t>
   </si>
 </sst>
 </file>
@@ -480,15 +495,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -505,131 +520,160 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>12</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>24</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D7" s="2">
         <v>3000</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="2">
-        <v>19800</v>
       </c>
       <c r="E7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="2">
+        <v>19800</v>
+      </c>
+      <c r="E8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>31</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>28</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="C5" r:id="rId4"/>
-    <hyperlink ref="C6" r:id="rId5"/>
-    <hyperlink ref="C7" r:id="rId6"/>
-    <hyperlink ref="C8" r:id="rId7"/>
+    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="C4" r:id="rId2"/>
+    <hyperlink ref="C5" r:id="rId3"/>
+    <hyperlink ref="C6" r:id="rId4"/>
+    <hyperlink ref="C7" r:id="rId5"/>
+    <hyperlink ref="C8" r:id="rId6"/>
+    <hyperlink ref="C9" r:id="rId7"/>
+    <hyperlink ref="C2" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>